<commit_message>
digital_elisa  from  excel  mode V1.0.1
</commit_message>
<xml_diff>
--- a/i_experimnet/files/info/root.xlsx
+++ b/i_experimnet/files/info/root.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/af369af656230de8/201.python/pythonWorkSpace/experiments_manager/i_experimnet/files/info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2BB1D69C5BA057F222104393473088B35299F1E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE2562E6-C0B4-4CA0-9B1C-A1DF0F58F94D}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_2BB1D69C5B30DB17A970A393593088B352998CDC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E20304D-419D-4FB5-9F36-97CB6ECD9502}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,15 +19,47 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>items</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>digital_elisa_protocol</t>
+  </si>
+  <si>
+    <t>../files/info/digital_elisa_protocol.xlsx</t>
+  </si>
+  <si>
+    <t>beads</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>../files/info/beads.xlsx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
@@ -45,7 +77,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -53,12 +85,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -361,15 +411,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D18"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>